<commit_message>
Ativ. 3 - Questão 6
</commit_message>
<xml_diff>
--- a/Pesquisa_Operacional/Atividade_3_Questao_6.xlsx
+++ b/Pesquisa_Operacional/Atividade_3_Questao_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\Notas_Aulas_ESOF\Pesquisa_Operacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150798EA-D5A0-4DE6-882E-D7824728F6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D39A3F-672A-4DD3-9647-DE26CD9D71CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19530" yWindow="0" windowWidth="16710" windowHeight="15600" xr2:uid="{382E2C25-C241-4AB8-8187-C97514301E0A}"/>
   </bookViews>
@@ -24,22 +24,25 @@
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">solver!$B$10</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">solver!$B$7:$B$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">solver!$B$2:$D$2</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">solver!$B$7:$B$9</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">solver!$B$4</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">solver!$D$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">solver!$D$7:$D$9</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">solver!$D$7:$D$9</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -217,9 +220,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -585,44 +591,51 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13">
+        <v>134</v>
+      </c>
+      <c r="C2" s="13">
+        <v>143</v>
+      </c>
+      <c r="D2" s="13">
+        <v>153</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <f>385*B2+329*C2+367.5*D2</f>
-        <v>0</v>
+        <v>154864.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -632,7 +645,7 @@
       </c>
       <c r="B7" s="1">
         <f>600*B2</f>
-        <v>0</v>
+        <v>80400</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -647,7 +660,7 @@
       </c>
       <c r="B8" s="1">
         <f>350*C2</f>
-        <v>0</v>
+        <v>50050</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -662,7 +675,7 @@
       </c>
       <c r="B9" s="1">
         <f>720*D2</f>
-        <v>0</v>
+        <v>110160</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -677,7 +690,7 @@
       </c>
       <c r="B10" s="1">
         <f>B2+C2+D2</f>
-        <v>0</v>
+        <v>430</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
@@ -710,198 +723,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>600</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="8">
         <v>5500</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="8">
         <v>80000</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <f>E4/C4</f>
         <v>133.33333333333334</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <f>0.07*D4</f>
         <v>385.00000000000006</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>350</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="8">
         <v>4700</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="8">
         <v>50000</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="8">
         <f t="shared" ref="F5:F6" si="0">E5/C5</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9">
         <f>0.07*D5</f>
         <v>329.00000000000006</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>720</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="8">
         <v>5250</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="8">
         <v>110000</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>152.77777777777777</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="9">
         <f>0.07*D6</f>
         <v>367.50000000000006</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="10">
         <v>450</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>